<commit_message>
Ajuste de bug da leitura dos meses e da geração do erro de falta de disciplina na fase
</commit_message>
<xml_diff>
--- a/src/modelo_cronograma/modelo_cronograma.xlsx
+++ b/src/modelo_cronograma/modelo_cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weber\OneDrive\Documentos\GitHub\TCS-BACK-END\src\modelo_cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F85057F-4EC8-48BE-ADFE-4AE2500F52EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41C8A58-BE68-47A5-8970-74C4F3534A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,6 +615,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -644,30 +668,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1049,10 +1049,10 @@
   <dimension ref="B1:AH50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H42" sqref="H42:AF47"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1111,34 +1111,34 @@
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="52"/>
-      <c r="W7" s="52"/>
-      <c r="X7" s="52"/>
-      <c r="Y7" s="52"/>
-      <c r="Z7" s="52"/>
-      <c r="AA7" s="52"/>
-      <c r="AB7" s="52"/>
-      <c r="AC7" s="52"/>
-      <c r="AD7" s="52"/>
-      <c r="AE7" s="52"/>
-      <c r="AF7" s="53"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="42"/>
+      <c r="V7" s="42"/>
+      <c r="W7" s="42"/>
+      <c r="X7" s="42"/>
+      <c r="Y7" s="42"/>
+      <c r="Z7" s="42"/>
+      <c r="AA7" s="42"/>
+      <c r="AB7" s="42"/>
+      <c r="AC7" s="42"/>
+      <c r="AD7" s="42"/>
+      <c r="AE7" s="42"/>
+      <c r="AF7" s="43"/>
     </row>
     <row r="8" spans="2:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
@@ -1150,34 +1150,34 @@
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
-      <c r="U8" s="54"/>
-      <c r="V8" s="54"/>
-      <c r="W8" s="54"/>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="54"/>
-      <c r="Z8" s="54"/>
-      <c r="AA8" s="54"/>
-      <c r="AB8" s="54"/>
-      <c r="AC8" s="54"/>
-      <c r="AD8" s="55"/>
-      <c r="AE8" s="55"/>
-      <c r="AF8" s="56"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="44"/>
+      <c r="W8" s="44"/>
+      <c r="X8" s="44"/>
+      <c r="Y8" s="44"/>
+      <c r="Z8" s="44"/>
+      <c r="AA8" s="44"/>
+      <c r="AB8" s="44"/>
+      <c r="AC8" s="44"/>
+      <c r="AD8" s="45"/>
+      <c r="AE8" s="45"/>
+      <c r="AF8" s="46"/>
     </row>
     <row r="9" spans="2:34" s="4" customFormat="1" ht="29.25" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
@@ -1198,46 +1198,46 @@
       <c r="G9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="H9" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="51"/>
-      <c r="J9" s="49" t="s">
+      <c r="I9" s="41"/>
+      <c r="J9" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="49" t="s">
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="50"/>
-      <c r="S9" s="51"/>
-      <c r="T9" s="49" t="s">
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="U9" s="50"/>
-      <c r="V9" s="50"/>
-      <c r="W9" s="50"/>
-      <c r="X9" s="50"/>
-      <c r="Y9" s="49" t="s">
+      <c r="U9" s="40"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="40"/>
+      <c r="Y9" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="Z9" s="50"/>
-      <c r="AA9" s="50"/>
-      <c r="AB9" s="50"/>
-      <c r="AC9" s="50"/>
-      <c r="AD9" s="49" t="s">
+      <c r="Z9" s="40"/>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="40"/>
+      <c r="AC9" s="40"/>
+      <c r="AD9" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="AE9" s="50"/>
-      <c r="AF9" s="51"/>
+      <c r="AE9" s="40"/>
+      <c r="AF9" s="41"/>
     </row>
     <row r="10" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="54" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="38"/>
@@ -1320,7 +1320,7 @@
       <c r="AH10"/>
     </row>
     <row r="11" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="47"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
       <c r="E11" s="38"/>
@@ -1401,7 +1401,7 @@
       <c r="AH11"/>
     </row>
     <row r="12" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="47"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
       <c r="E12" s="38"/>
@@ -1482,7 +1482,7 @@
       <c r="AH12"/>
     </row>
     <row r="13" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="47"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
@@ -1561,7 +1561,7 @@
       </c>
     </row>
     <row r="14" spans="2:34" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="47"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
@@ -1640,7 +1640,7 @@
       </c>
     </row>
     <row r="15" spans="2:34" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="48"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -1787,7 +1787,7 @@
       <c r="AH17" s="11"/>
     </row>
     <row r="18" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="50" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="38"/>
@@ -1870,7 +1870,7 @@
       <c r="AH18"/>
     </row>
     <row r="19" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="42"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="38"/>
       <c r="D19" s="38"/>
       <c r="E19" s="38"/>
@@ -1951,7 +1951,7 @@
       <c r="AH19"/>
     </row>
     <row r="20" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="42"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
       <c r="E20" s="38"/>
@@ -2032,7 +2032,7 @@
       <c r="AH20"/>
     </row>
     <row r="21" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="43"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
@@ -2111,7 +2111,7 @@
       </c>
     </row>
     <row r="22" spans="2:34" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="43"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
       <c r="E22" s="38"/>
@@ -2190,7 +2190,7 @@
       </c>
     </row>
     <row r="23" spans="2:34" s="17" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="43"/>
+      <c r="B23" s="51"/>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -2337,7 +2337,7 @@
       <c r="AH25" s="11"/>
     </row>
     <row r="26" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="52" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="38"/>
@@ -2420,7 +2420,7 @@
       <c r="AH26"/>
     </row>
     <row r="27" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="45"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
@@ -2501,7 +2501,7 @@
       <c r="AH27"/>
     </row>
     <row r="28" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="40"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
@@ -2582,7 +2582,7 @@
       <c r="AH28"/>
     </row>
     <row r="29" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="40"/>
+      <c r="B29" s="48"/>
       <c r="C29" s="38"/>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
@@ -2661,7 +2661,7 @@
       </c>
     </row>
     <row r="30" spans="2:34" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="40"/>
+      <c r="B30" s="48"/>
       <c r="C30" s="38"/>
       <c r="D30" s="38"/>
       <c r="E30" s="38"/>
@@ -2740,7 +2740,7 @@
       </c>
     </row>
     <row r="31" spans="2:34" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B31" s="41"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="27"/>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
@@ -2887,7 +2887,7 @@
       <c r="AH33" s="11"/>
     </row>
     <row r="34" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="47" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="38"/>
@@ -2970,7 +2970,7 @@
       <c r="AH34"/>
     </row>
     <row r="35" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="40"/>
+      <c r="B35" s="48"/>
       <c r="C35" s="38"/>
       <c r="D35" s="38"/>
       <c r="E35" s="38"/>
@@ -3051,7 +3051,7 @@
       <c r="AH35"/>
     </row>
     <row r="36" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="40"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="38"/>
       <c r="D36" s="38"/>
       <c r="E36" s="38"/>
@@ -3132,7 +3132,7 @@
       <c r="AH36"/>
     </row>
     <row r="37" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="40"/>
+      <c r="B37" s="48"/>
       <c r="C37" s="38"/>
       <c r="D37" s="38"/>
       <c r="E37" s="38"/>
@@ -3211,7 +3211,7 @@
       </c>
     </row>
     <row r="38" spans="2:34" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="40"/>
+      <c r="B38" s="48"/>
       <c r="C38" s="38"/>
       <c r="D38" s="38"/>
       <c r="E38" s="38"/>
@@ -3290,7 +3290,7 @@
       </c>
     </row>
     <row r="39" spans="2:34" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B39" s="41"/>
+      <c r="B39" s="49"/>
       <c r="C39" s="27"/>
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
@@ -3381,7 +3381,7 @@
       <c r="F41" s="26"/>
     </row>
     <row r="42" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="39" t="s">
+      <c r="B42" s="47" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="38"/>
@@ -3464,7 +3464,7 @@
       <c r="AH42"/>
     </row>
     <row r="43" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="40"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="38"/>
       <c r="D43" s="38"/>
       <c r="E43" s="38"/>
@@ -3545,7 +3545,7 @@
       <c r="AH43"/>
     </row>
     <row r="44" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="40"/>
+      <c r="B44" s="48"/>
       <c r="C44" s="38"/>
       <c r="D44" s="38"/>
       <c r="E44" s="38"/>
@@ -3626,7 +3626,7 @@
       <c r="AH44"/>
     </row>
     <row r="45" spans="2:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="40"/>
+      <c r="B45" s="48"/>
       <c r="C45" s="38"/>
       <c r="D45" s="38"/>
       <c r="E45" s="38"/>
@@ -3705,7 +3705,7 @@
       </c>
     </row>
     <row r="46" spans="2:34" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="40"/>
+      <c r="B46" s="48"/>
       <c r="C46" s="38"/>
       <c r="D46" s="38"/>
       <c r="E46" s="38"/>
@@ -3784,7 +3784,7 @@
       </c>
     </row>
     <row r="47" spans="2:34" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B47" s="41"/>
+      <c r="B47" s="49"/>
       <c r="C47" s="27"/>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
@@ -3882,6 +3882,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="B10:B15"/>
     <mergeCell ref="J9:N9"/>
     <mergeCell ref="O9:S9"/>
     <mergeCell ref="T9:X9"/>
@@ -3890,11 +3895,6 @@
     <mergeCell ref="Y9:AC9"/>
     <mergeCell ref="AD9:AF9"/>
     <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B42:B47"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="B10:B15"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.27559055118110237" top="0.67" bottom="0.23622047244094491" header="0.27559055118110237" footer="0"/>

</xml_diff>